<commit_message>
feat: update i18n docs
</commit_message>
<xml_diff>
--- a/docs/lang.xlsx
+++ b/docs/lang.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>key</t>
   </si>
@@ -36,10 +36,7 @@
     </r>
   </si>
   <si>
-    <t>请选择</t>
-  </si>
-  <si>
-    <t>Select</t>
+    <t>{msg} world</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -621,7 +618,7 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1376,7 +1373,7 @@
   <dimension ref="A1:K667"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1414,7 +1411,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
@@ -1725,7 +1722,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" ht="49.5" spans="4:11">
+    <row r="33" ht="16.5" spans="4:11">
       <c r="D33" s="11"/>
       <c r="E33" s="1"/>
       <c r="F33" s="7"/>
@@ -2617,7 +2614,7 @@
     </row>
     <row r="122" ht="16.5" spans="4:11">
       <c r="D122" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="11"/>
@@ -3099,7 +3096,7 @@
     </row>
     <row r="170" ht="16.5" spans="4:11">
       <c r="D170" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="11"/>
@@ -7341,7 +7338,7 @@
     </row>
     <row r="594" ht="16.5" spans="4:11">
       <c r="D594" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E594" s="1"/>
       <c r="F594" s="11"/>
@@ -7373,7 +7370,7 @@
     </row>
     <row r="597" ht="16.5" spans="4:11">
       <c r="D597" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E597" s="1"/>
       <c r="F597" s="11"/>

</xml_diff>

<commit_message>
feat: dev router func
</commit_message>
<xml_diff>
--- a/docs/lang.xlsx
+++ b/docs/lang.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>key</t>
   </si>
@@ -34,6 +34,9 @@
       </rPr>
       <t>trans0001</t>
     </r>
+  </si>
+  <si>
+    <t>{msg} 世界</t>
   </si>
   <si>
     <t>{msg} world</t>
@@ -1373,7 +1376,7 @@
   <dimension ref="A1:K667"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1411,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="122" ht="16.5" spans="4:11">
       <c r="D122" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="11"/>
@@ -3096,7 +3099,7 @@
     </row>
     <row r="170" ht="16.5" spans="4:11">
       <c r="D170" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="11"/>
@@ -7338,7 +7341,7 @@
     </row>
     <row r="594" ht="16.5" spans="4:11">
       <c r="D594" s="21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E594" s="1"/>
       <c r="F594" s="11"/>
@@ -7370,7 +7373,7 @@
     </row>
     <row r="597" ht="16.5" spans="4:11">
       <c r="D597" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E597" s="1"/>
       <c r="F597" s="11"/>

</xml_diff>

<commit_message>
feat: add userForm hook
</commit_message>
<xml_diff>
--- a/docs/lang.xlsx
+++ b/docs/lang.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>key</t>
   </si>
@@ -242,10 +242,67 @@
     <t>trans0024</t>
   </si>
   <si>
+    <t>登录</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
     <t>trans0025</t>
   </si>
   <si>
+    <t>邮箱</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>trans0026</t>
+  </si>
+  <si>
+    <t>密码</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>trans0027</t>
+  </si>
+  <si>
+    <t>忘记密码？</t>
+  </si>
+  <si>
+    <t>Forget Password?</t>
+  </si>
+  <si>
+    <t>trans0028</t>
+  </si>
+  <si>
+    <t>记住我</t>
+  </si>
+  <si>
+    <t>Remember me</t>
+  </si>
+  <si>
+    <t>trans0029</t>
+  </si>
+  <si>
+    <t>请输入{val}</t>
+  </si>
+  <si>
+    <t>Please input {val}</t>
+  </si>
+  <si>
+    <t>trans0030</t>
+  </si>
+  <si>
+    <t>trans0031</t>
+  </si>
+  <si>
+    <t>trans0032</t>
+  </si>
+  <si>
+    <t>trans0033</t>
   </si>
 </sst>
 </file>
@@ -1600,8 +1657,8 @@
   <sheetPr/>
   <dimension ref="A1:K667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A575" workbookViewId="0">
-      <selection activeCell="E588" sqref="E588"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2072,6 +2129,12 @@
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="B25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>
       <c r="F25" s="10"/>
@@ -2083,7 +2146,13 @@
     </row>
     <row r="26" ht="17.25" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="1"/>
@@ -2096,7 +2165,13 @@
     </row>
     <row r="27" ht="16.5" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="1"/>
@@ -2107,7 +2182,16 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" ht="16.5" spans="4:11">
+    <row r="28" ht="16.5" spans="1:11">
+      <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="D28" s="7"/>
       <c r="E28" s="1"/>
       <c r="F28" s="10"/>
@@ -2117,7 +2201,16 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" ht="16.5" spans="4:11">
+    <row r="29" ht="16.5" spans="1:11">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="1"/>
       <c r="F29" s="10"/>
@@ -2127,7 +2220,16 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" ht="16.5" spans="4:11">
+    <row r="30" ht="16.5" spans="1:11">
+      <c r="A30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="D30" s="7"/>
       <c r="E30" s="1"/>
       <c r="F30" s="10"/>
@@ -2137,7 +2239,10 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" ht="16.5" spans="4:11">
+    <row r="31" ht="16.5" spans="1:11">
+      <c r="A31" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="D31" s="7"/>
       <c r="E31" s="1"/>
       <c r="F31" s="10"/>
@@ -2147,7 +2252,10 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" ht="16.5" spans="4:11">
+    <row r="32" ht="16.5" spans="1:11">
+      <c r="A32" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="D32" s="7"/>
       <c r="E32" s="1"/>
       <c r="F32" s="10"/>
@@ -2157,7 +2265,10 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" ht="16.5" spans="4:11">
+    <row r="33" ht="16.5" spans="1:11">
+      <c r="A33" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D33" s="14"/>
       <c r="E33" s="1"/>
       <c r="F33" s="10"/>
@@ -2167,7 +2278,10 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" ht="16.5" spans="4:11">
+    <row r="34" ht="16.5" spans="1:11">
+      <c r="A34" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D34" s="7"/>
       <c r="E34" s="1"/>
       <c r="F34" s="10"/>

</xml_diff>

<commit_message>
feat: add theme toggle
</commit_message>
<xml_diff>
--- a/docs/lang.xlsx
+++ b/docs/lang.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>key</t>
   </si>
@@ -296,10 +296,28 @@
     <t>trans0030</t>
   </si>
   <si>
+    <t>暗色模式</t>
+  </si>
+  <si>
+    <t>Dark Mode</t>
+  </si>
+  <si>
     <t>trans0031</t>
   </si>
   <si>
+    <t>亮色模式</t>
+  </si>
+  <si>
+    <t>Light Mode</t>
+  </si>
+  <si>
     <t>trans0032</t>
+  </si>
+  <si>
+    <t>自动模式</t>
+  </si>
+  <si>
+    <t>Automatic Mode</t>
   </si>
   <si>
     <t>trans0033</t>
@@ -1658,7 +1676,7 @@
   <dimension ref="A1:K667"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2243,6 +2261,12 @@
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="B31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D31" s="7"/>
       <c r="E31" s="1"/>
       <c r="F31" s="10"/>
@@ -2254,7 +2278,13 @@
     </row>
     <row r="32" ht="16.5" spans="1:11">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="1"/>
@@ -2267,7 +2297,13 @@
     </row>
     <row r="33" ht="16.5" spans="1:11">
       <c r="A33" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="1"/>
@@ -2280,7 +2316,7 @@
     </row>
     <row r="34" ht="16.5" spans="1:11">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="1"/>

</xml_diff>